<commit_message>
baby analysis + next exp
</commit_message>
<xml_diff>
--- a/baby_analysis/data/output.xlsx
+++ b/baby_analysis/data/output.xlsx
@@ -59,6 +59,10 @@
     <sheet state="visible" name="28_2" sheetId="54" r:id="rId57"/>
     <sheet state="visible" name="30_1" sheetId="55" r:id="rId58"/>
     <sheet state="visible" name="30_2" sheetId="56" r:id="rId59"/>
+    <sheet state="visible" name="31_1" sheetId="57" r:id="rId60"/>
+    <sheet state="visible" name="33_1" sheetId="58" r:id="rId61"/>
+    <sheet state="visible" name="34_1" sheetId="59" r:id="rId62"/>
+    <sheet state="visible" name="35_1" sheetId="60" r:id="rId63"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -66,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1722" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="22">
   <si>
     <t>Trial Number</t>
   </si>
@@ -313,11 +317,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="51308188"/>
-        <c:axId val="1512673847"/>
+        <c:axId val="1193938744"/>
+        <c:axId val="1969205473"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51308188"/>
+        <c:axId val="1193938744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -369,10 +373,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1512673847"/>
+        <c:crossAx val="1969205473"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1512673847"/>
+        <c:axId val="1969205473"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -447,7 +451,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51308188"/>
+        <c:crossAx val="1193938744"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -542,11 +546,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="444689178"/>
-        <c:axId val="1028613927"/>
+        <c:axId val="279745605"/>
+        <c:axId val="2105350564"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="444689178"/>
+        <c:axId val="279745605"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,10 +602,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1028613927"/>
+        <c:crossAx val="2105350564"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1028613927"/>
+        <c:axId val="2105350564"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -676,7 +680,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="444689178"/>
+        <c:crossAx val="279745605"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -962,7 +966,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing57.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing58.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing59.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing60.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -43745,6 +43765,3069 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1.959</v>
+      </c>
+      <c r="E2" s="8">
+        <v>4.743</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>1.959</v>
+      </c>
+      <c r="H2" s="8">
+        <v>4.743</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1.959</v>
+      </c>
+      <c r="K2" s="8">
+        <v>4.743</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="8">
+        <v>1.959</v>
+      </c>
+      <c r="N2" s="8">
+        <v>4.743</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P2" s="8">
+        <v>1.959</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>4.743</v>
+      </c>
+      <c r="R2" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8">
+        <v>43.997</v>
+      </c>
+      <c r="E3" s="8">
+        <v>9.277</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>35.839</v>
+      </c>
+      <c r="H3" s="8">
+        <v>5.159</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>35.839</v>
+      </c>
+      <c r="K3" s="8">
+        <v>5.159</v>
+      </c>
+      <c r="L3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="8">
+        <v>35.839</v>
+      </c>
+      <c r="N3" s="8">
+        <v>5.159</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P3" s="8">
+        <v>35.839</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>5.159</v>
+      </c>
+      <c r="R3" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8">
+        <v>11.279</v>
+      </c>
+      <c r="E4" s="8">
+        <v>11.718</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="H4" s="8">
+        <v>6.439</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>6.439</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="N4" s="8">
+        <v>6.439</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>6.439</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4.799</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.479</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4.799</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.479</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>4.799</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.479</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>4.799</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0.479</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="8">
+        <v>4.799</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0.479</v>
+      </c>
+      <c r="R5" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>40.719</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>40.719</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>40.719</v>
+      </c>
+      <c r="K6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>40.719</v>
+      </c>
+      <c r="N6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P6" s="8">
+        <v>40.719</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R6" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>33.635</v>
+      </c>
+      <c r="E7" s="8">
+        <v>12.315</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>20.839</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2.639</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>20.839</v>
+      </c>
+      <c r="K7" s="8">
+        <v>2.639</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>20.839</v>
+      </c>
+      <c r="N7" s="8">
+        <v>2.639</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P7" s="8">
+        <v>33.635</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>12.315</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2.959</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>2.959</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>2.959</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>2.959</v>
+      </c>
+      <c r="N8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="8">
+        <v>2.959</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8">
+        <v>36.758</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2.759</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>31.319</v>
+      </c>
+      <c r="H9" s="8">
+        <v>2.759</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="8">
+        <v>31.319</v>
+      </c>
+      <c r="K9" s="8">
+        <v>2.759</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>31.319</v>
+      </c>
+      <c r="N9" s="8">
+        <v>2.759</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P9" s="8">
+        <v>31.319</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>2.759</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8">
+        <v>14.839</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>14.839</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>14.839</v>
+      </c>
+      <c r="K10" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="8">
+        <v>14.839</v>
+      </c>
+      <c r="N10" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P10" s="8">
+        <v>14.839</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="R10" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8">
+        <v>4.398</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2.039</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="H11" s="8">
+        <v>2.039</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J11" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="K11" s="8">
+        <v>2.039</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="N11" s="8">
+        <v>2.039</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P11" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>2.039</v>
+      </c>
+      <c r="R11" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8">
+        <v>20.158</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>15.439</v>
+      </c>
+      <c r="H12" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>15.439</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>15.439</v>
+      </c>
+      <c r="N12" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P12" s="8">
+        <v>15.439</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="R12" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3.999</v>
+      </c>
+      <c r="E13" s="8">
+        <v>10.398</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>3.999</v>
+      </c>
+      <c r="H13" s="8">
+        <v>10.398</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>3.999</v>
+      </c>
+      <c r="K13" s="8">
+        <v>10.398</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>3.999</v>
+      </c>
+      <c r="N13" s="8">
+        <v>10.398</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>3.999</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>10.398</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P14" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8">
+        <v>15.837</v>
+      </c>
+      <c r="E15" s="8">
+        <v>7.118</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>6.119</v>
+      </c>
+      <c r="H15" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>6.119</v>
+      </c>
+      <c r="K15" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>6.119</v>
+      </c>
+      <c r="N15" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P15" s="8">
+        <v>6.119</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="R15" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="8">
+        <v>4.918</v>
+      </c>
+      <c r="E16" s="8">
+        <v>7.879</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>3.639</v>
+      </c>
+      <c r="H16" s="8">
+        <v>7.879</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>3.639</v>
+      </c>
+      <c r="K16" s="8">
+        <v>7.879</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="8">
+        <v>3.639</v>
+      </c>
+      <c r="N16" s="8">
+        <v>7.879</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>3.639</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>7.879</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1.146</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1.146</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="K2" s="8">
+        <v>1.146</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="N2" s="8">
+        <v>1.146</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P2" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>1.146</v>
+      </c>
+      <c r="R2" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8">
+        <v>21.634</v>
+      </c>
+      <c r="E3" s="8">
+        <v>17.475</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>8.478</v>
+      </c>
+      <c r="H3" s="8">
+        <v>8.558</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>8.478</v>
+      </c>
+      <c r="K3" s="8">
+        <v>8.558</v>
+      </c>
+      <c r="L3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="8">
+        <v>8.478</v>
+      </c>
+      <c r="N3" s="8">
+        <v>8.558</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P3" s="8">
+        <v>8.478</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>8.558</v>
+      </c>
+      <c r="R3" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8">
+        <v>9.678</v>
+      </c>
+      <c r="E4" s="8">
+        <v>3.719</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>8.639</v>
+      </c>
+      <c r="H4" s="8">
+        <v>3.719</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="8">
+        <v>8.639</v>
+      </c>
+      <c r="K4" s="8">
+        <v>3.719</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="8">
+        <v>8.639</v>
+      </c>
+      <c r="N4" s="8">
+        <v>3.719</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P4" s="8">
+        <v>8.639</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>3.719</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R5" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>26.753</v>
+      </c>
+      <c r="E6" s="8">
+        <v>27.153</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>10.878</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3.038</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>10.878</v>
+      </c>
+      <c r="K6" s="8">
+        <v>3.038</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>17.397</v>
+      </c>
+      <c r="N6" s="8">
+        <v>7.997</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P6" s="8">
+        <v>17.397</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>7.997</v>
+      </c>
+      <c r="R6" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.758</v>
+      </c>
+      <c r="E7" s="8">
+        <v>8.638</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0.519</v>
+      </c>
+      <c r="H7" s="8">
+        <v>8.638</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>0.519</v>
+      </c>
+      <c r="K7" s="8">
+        <v>8.638</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>0.519</v>
+      </c>
+      <c r="N7" s="8">
+        <v>8.638</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P7" s="8">
+        <v>0.519</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>8.638</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8">
+        <v>5.679</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>5.679</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>5.679</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>5.679</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="8">
+        <v>5.679</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8">
+        <v>13.235</v>
+      </c>
+      <c r="E9" s="8">
+        <v>9.076</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>7.439</v>
+      </c>
+      <c r="H9" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="8">
+        <v>7.439</v>
+      </c>
+      <c r="K9" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>7.439</v>
+      </c>
+      <c r="N9" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P9" s="8">
+        <v>7.439</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8">
+        <v>7.156</v>
+      </c>
+      <c r="E10" s="8">
+        <v>11.676</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>3.279</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>3.279</v>
+      </c>
+      <c r="K10" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="8">
+        <v>3.279</v>
+      </c>
+      <c r="N10" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P10" s="8">
+        <v>5.037</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>7.997</v>
+      </c>
+      <c r="R10" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.239</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.239</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J11" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.239</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.239</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P11" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0.239</v>
+      </c>
+      <c r="R11" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8">
+        <v>13.635</v>
+      </c>
+      <c r="E12" s="8">
+        <v>8.275</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="H12" s="8">
+        <v>2.319</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2.319</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="N12" s="8">
+        <v>2.319</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P12" s="8">
+        <v>4.159</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>2.319</v>
+      </c>
+      <c r="R12" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3.037</v>
+      </c>
+      <c r="E13" s="8">
+        <v>11.316</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>1.279</v>
+      </c>
+      <c r="H13" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1.279</v>
+      </c>
+      <c r="K13" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>1.279</v>
+      </c>
+      <c r="N13" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>1.279</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="8">
+        <v>4.759</v>
+      </c>
+      <c r="E14" s="8">
+        <v>1.599</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>4.759</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1.599</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>4.759</v>
+      </c>
+      <c r="K14" s="8">
+        <v>1.599</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>4.759</v>
+      </c>
+      <c r="N14" s="8">
+        <v>1.599</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P14" s="8">
+        <v>4.759</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>1.599</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8">
+        <v>17.553</v>
+      </c>
+      <c r="E15" s="8">
+        <v>33.513</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>3.919</v>
+      </c>
+      <c r="H15" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>3.919</v>
+      </c>
+      <c r="K15" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>3.919</v>
+      </c>
+      <c r="N15" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P15" s="8">
+        <v>3.919</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>3.119</v>
+      </c>
+      <c r="R15" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="8">
+        <v>13.395</v>
+      </c>
+      <c r="E16" s="8">
+        <v>12.395</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>5.838</v>
+      </c>
+      <c r="H16" s="8">
+        <v>5.957</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>5.838</v>
+      </c>
+      <c r="K16" s="8">
+        <v>5.957</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="8">
+        <v>12.316</v>
+      </c>
+      <c r="N16" s="8">
+        <v>12.395</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>12.316</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>12.395</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="8">
+        <v>8.239</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>8.239</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>8.239</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>8.239</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P17" s="8">
+        <v>8.239</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R17" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="8">
+        <v>21.514</v>
+      </c>
+      <c r="E18" s="8">
+        <v>18.554</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="H18" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="K18" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M18" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="N18" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="O18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P18" s="8">
+        <v>4.519</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="R18" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0.958</v>
+      </c>
+      <c r="E19" s="8">
+        <v>7.997</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="H19" s="8">
+        <v>6.838</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J19" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="K19" s="8">
+        <v>6.838</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M19" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="N19" s="8">
+        <v>6.838</v>
+      </c>
+      <c r="O19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P19" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>6.838</v>
+      </c>
+      <c r="R19" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8">
+        <v>6.323</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>6.323</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="8">
+        <v>6.323</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="8">
+        <v>6.323</v>
+      </c>
+      <c r="N2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P2" s="8">
+        <v>6.323</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R2" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8">
+        <v>38.039</v>
+      </c>
+      <c r="E3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>38.039</v>
+      </c>
+      <c r="H3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>38.039</v>
+      </c>
+      <c r="K3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="8">
+        <v>38.039</v>
+      </c>
+      <c r="N3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P3" s="8">
+        <v>38.039</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R3" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8">
+        <v>31.757</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2.439</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="G4" s="8">
+        <v>30.998</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2.439</v>
+      </c>
+      <c r="I4" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="J4" s="8">
+        <v>30.998</v>
+      </c>
+      <c r="K4" s="8">
+        <v>2.439</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="M4" s="8">
+        <v>30.998</v>
+      </c>
+      <c r="N4" s="8">
+        <v>2.439</v>
+      </c>
+      <c r="O4" s="8">
+        <v>1.399</v>
+      </c>
+      <c r="P4" s="8">
+        <v>30.998</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>2.439</v>
+      </c>
+      <c r="R4" s="8">
+        <v>1.399</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="K5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="N5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="8">
+        <v>4.959</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R5" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>36.558</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1.639</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1.119</v>
+      </c>
+      <c r="G6" s="8">
+        <v>36.558</v>
+      </c>
+      <c r="H6" s="8">
+        <v>1.639</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1.119</v>
+      </c>
+      <c r="J6" s="8">
+        <v>36.558</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1.639</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1.119</v>
+      </c>
+      <c r="M6" s="8">
+        <v>36.558</v>
+      </c>
+      <c r="N6" s="8">
+        <v>1.639</v>
+      </c>
+      <c r="O6" s="8">
+        <v>1.119</v>
+      </c>
+      <c r="P6" s="8">
+        <v>36.558</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>1.639</v>
+      </c>
+      <c r="R6" s="8">
+        <v>1.119</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>12.278</v>
+      </c>
+      <c r="E7" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="F7" s="8">
+        <v>8.319</v>
+      </c>
+      <c r="G7" s="8">
+        <v>12.278</v>
+      </c>
+      <c r="H7" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="I7" s="8">
+        <v>8.319</v>
+      </c>
+      <c r="J7" s="8">
+        <v>12.278</v>
+      </c>
+      <c r="K7" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="L7" s="8">
+        <v>8.319</v>
+      </c>
+      <c r="M7" s="8">
+        <v>12.278</v>
+      </c>
+      <c r="N7" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="O7" s="8">
+        <v>8.319</v>
+      </c>
+      <c r="P7" s="8">
+        <v>12.278</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0.879</v>
+      </c>
+      <c r="R7" s="8">
+        <v>8.319</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8">
+        <v>15.878</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3.158</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>12.319</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>12.319</v>
+      </c>
+      <c r="K8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>12.319</v>
+      </c>
+      <c r="N8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="8">
+        <v>12.319</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8">
+        <v>23.394</v>
+      </c>
+      <c r="E9" s="8">
+        <v>31.473</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>7.519</v>
+      </c>
+      <c r="H9" s="8">
+        <v>11.518</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="8">
+        <v>7.519</v>
+      </c>
+      <c r="K9" s="8">
+        <v>11.518</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>7.519</v>
+      </c>
+      <c r="N9" s="8">
+        <v>11.518</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P9" s="8">
+        <v>7.519</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>11.518</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="E10" s="8">
+        <v>4.238</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="H10" s="8">
+        <v>4.238</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="K10" s="8">
+        <v>4.238</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="N10" s="8">
+        <v>4.238</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P10" s="8">
+        <v>9.919</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>4.238</v>
+      </c>
+      <c r="R10" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8">
+        <v>37.396</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4.516</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>32.517</v>
+      </c>
+      <c r="H11" s="8">
+        <v>4.516</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J11" s="8">
+        <v>32.517</v>
+      </c>
+      <c r="K11" s="8">
+        <v>4.516</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>32.517</v>
+      </c>
+      <c r="N11" s="8">
+        <v>4.516</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P11" s="8">
+        <v>32.517</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>4.516</v>
+      </c>
+      <c r="R11" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8">
+        <v>17.998</v>
+      </c>
+      <c r="E12" s="8">
+        <v>4.119</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="H12" s="8">
+        <v>4.119</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="K12" s="8">
+        <v>4.119</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="N12" s="8">
+        <v>4.119</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P12" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>4.119</v>
+      </c>
+      <c r="R12" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8">
+        <v>18.195</v>
+      </c>
+      <c r="E13" s="8">
+        <v>8.276</v>
+      </c>
+      <c r="F13" s="8">
+        <v>2.479</v>
+      </c>
+      <c r="G13" s="8">
+        <v>8.879</v>
+      </c>
+      <c r="H13" s="8">
+        <v>3.319</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>8.879</v>
+      </c>
+      <c r="K13" s="8">
+        <v>3.319</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>8.879</v>
+      </c>
+      <c r="N13" s="8">
+        <v>3.319</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>8.879</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>3.319</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="8">
+        <v>5.479</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>5.479</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>5.479</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>5.479</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P14" s="8">
+        <v>5.479</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8">
+        <v>10.797</v>
+      </c>
+      <c r="E15" s="8">
+        <v>14.397</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>6.639</v>
+      </c>
+      <c r="H15" s="8">
+        <v>4.359</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>6.639</v>
+      </c>
+      <c r="K15" s="8">
+        <v>4.359</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>6.639</v>
+      </c>
+      <c r="N15" s="8">
+        <v>4.359</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P15" s="8">
+        <v>6.639</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>4.359</v>
+      </c>
+      <c r="R15" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="8">
+        <v>17.638</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3.638</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>7.039</v>
+      </c>
+      <c r="H16" s="8">
+        <v>3.638</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>7.039</v>
+      </c>
+      <c r="K16" s="8">
+        <v>3.638</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="8">
+        <v>7.039</v>
+      </c>
+      <c r="N16" s="8">
+        <v>3.638</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>7.039</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>3.638</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="8">
+        <v>8.799</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>8.799</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>8.799</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>8.799</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P17" s="8">
+        <v>8.799</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R17" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="8">
+        <v>28.114</v>
+      </c>
+      <c r="E18" s="8">
+        <v>27.034</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="H18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="K18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="N18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="O18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>12.199</v>
+      </c>
+      <c r="R18" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="E19" s="8">
+        <v>4.358</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G19" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="H19" s="8">
+        <v>4.358</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J19" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="K19" s="8">
+        <v>4.358</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M19" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="N19" s="8">
+        <v>4.358</v>
+      </c>
+      <c r="O19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P19" s="8">
+        <v>9.079</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>4.358</v>
+      </c>
+      <c r="R19" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
@@ -44814,6 +47897,1083 @@
         <v>4.84</v>
       </c>
       <c r="R19" s="4">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1.0</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J2" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="K2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M2" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="N2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P2" s="8">
+        <v>4.999</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R2" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="B3" s="8">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="8">
+        <v>13.915</v>
+      </c>
+      <c r="E3" s="8">
+        <v>8.996</v>
+      </c>
+      <c r="F3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="H3" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="I3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J3" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="K3" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="L3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M3" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="N3" s="8">
+        <v>2.599</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P3" s="8">
+        <v>12.396</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>8.996</v>
+      </c>
+      <c r="R3" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8">
+        <v>27.278</v>
+      </c>
+      <c r="E4" s="8">
+        <v>5.878</v>
+      </c>
+      <c r="F4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>6.479</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1.679</v>
+      </c>
+      <c r="I4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J4" s="8">
+        <v>27.278</v>
+      </c>
+      <c r="K4" s="8">
+        <v>5.878</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M4" s="8">
+        <v>27.278</v>
+      </c>
+      <c r="N4" s="8">
+        <v>5.878</v>
+      </c>
+      <c r="O4" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P4" s="8">
+        <v>27.278</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>5.878</v>
+      </c>
+      <c r="R4" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="B5" s="8">
+        <v>4.0</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>4.239</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="8">
+        <v>4.239</v>
+      </c>
+      <c r="H5" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="I5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J5" s="8">
+        <v>4.239</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="L5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M5" s="8">
+        <v>4.239</v>
+      </c>
+      <c r="N5" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="O5" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P5" s="8">
+        <v>4.239</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>2.519</v>
+      </c>
+      <c r="R5" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="B6" s="8">
+        <v>5.0</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="8">
+        <v>29.873</v>
+      </c>
+      <c r="E6" s="8">
+        <v>23.433</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>5.199</v>
+      </c>
+      <c r="H6" s="8">
+        <v>3.039</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="8">
+        <v>5.199</v>
+      </c>
+      <c r="K6" s="8">
+        <v>3.039</v>
+      </c>
+      <c r="L6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M6" s="8">
+        <v>5.199</v>
+      </c>
+      <c r="N6" s="8">
+        <v>3.039</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P6" s="8">
+        <v>5.199</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>3.039</v>
+      </c>
+      <c r="R6" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="B7" s="8">
+        <v>6.0</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="8">
+        <v>13.196</v>
+      </c>
+      <c r="E7" s="8">
+        <v>4.996</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>5.199</v>
+      </c>
+      <c r="H7" s="8">
+        <v>5.958</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J7" s="8">
+        <v>8.798</v>
+      </c>
+      <c r="K7" s="8">
+        <v>8.517</v>
+      </c>
+      <c r="L7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M7" s="8">
+        <v>8.798</v>
+      </c>
+      <c r="N7" s="8">
+        <v>8.517</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P7" s="8">
+        <v>8.798</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>8.517</v>
+      </c>
+      <c r="R7" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="B8" s="8">
+        <v>7.0</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J8" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="K8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M8" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="N8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P8" s="8">
+        <v>5.839</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R8" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="B9" s="8">
+        <v>8.0</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="8">
+        <v>27.835</v>
+      </c>
+      <c r="E9" s="8">
+        <v>9.075</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G9" s="8">
+        <v>10.598</v>
+      </c>
+      <c r="H9" s="8">
+        <v>4.318</v>
+      </c>
+      <c r="I9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J9" s="8">
+        <v>10.598</v>
+      </c>
+      <c r="K9" s="8">
+        <v>4.318</v>
+      </c>
+      <c r="L9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M9" s="8">
+        <v>10.598</v>
+      </c>
+      <c r="N9" s="8">
+        <v>4.318</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P9" s="8">
+        <v>10.598</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>4.318</v>
+      </c>
+      <c r="R9" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="B10" s="8">
+        <v>9.0</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="8">
+        <v>11.195</v>
+      </c>
+      <c r="E10" s="8">
+        <v>18.675</v>
+      </c>
+      <c r="F10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>5.319</v>
+      </c>
+      <c r="H10" s="8">
+        <v>7.198</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J10" s="8">
+        <v>5.319</v>
+      </c>
+      <c r="K10" s="8">
+        <v>7.198</v>
+      </c>
+      <c r="L10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M10" s="8">
+        <v>5.319</v>
+      </c>
+      <c r="N10" s="8">
+        <v>7.198</v>
+      </c>
+      <c r="O10" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P10" s="8">
+        <v>5.319</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>7.198</v>
+      </c>
+      <c r="R10" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="B11" s="8">
+        <v>10.0</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="8">
+        <v>9.83</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="8">
+        <v>9.83</v>
+      </c>
+      <c r="H11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J11" s="8">
+        <v>9.83</v>
+      </c>
+      <c r="K11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M11" s="8">
+        <v>9.83</v>
+      </c>
+      <c r="N11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P11" s="8">
+        <v>9.83</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R11" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="B12" s="8">
+        <v>11.0</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="8">
+        <v>23.714</v>
+      </c>
+      <c r="E12" s="8">
+        <v>15.354</v>
+      </c>
+      <c r="F12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>5.759</v>
+      </c>
+      <c r="H12" s="8">
+        <v>2.079</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J12" s="8">
+        <v>5.759</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2.079</v>
+      </c>
+      <c r="L12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M12" s="8">
+        <v>12.277</v>
+      </c>
+      <c r="N12" s="8">
+        <v>6.197</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P12" s="8">
+        <v>23.115</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>14.395</v>
+      </c>
+      <c r="R12" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="B13" s="8">
+        <v>12.0</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="8">
+        <v>4.677</v>
+      </c>
+      <c r="E13" s="8">
+        <v>13.436</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.079</v>
+      </c>
+      <c r="H13" s="8">
+        <v>7.878</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0.079</v>
+      </c>
+      <c r="K13" s="8">
+        <v>7.878</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0.079</v>
+      </c>
+      <c r="N13" s="8">
+        <v>7.878</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P13" s="8">
+        <v>0.079</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>7.878</v>
+      </c>
+      <c r="R13" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="B14" s="8">
+        <v>13.0</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="8">
+        <v>5.599</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>5.599</v>
+      </c>
+      <c r="H14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J14" s="8">
+        <v>5.599</v>
+      </c>
+      <c r="K14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M14" s="8">
+        <v>5.599</v>
+      </c>
+      <c r="N14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P14" s="8">
+        <v>5.599</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R14" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="B15" s="8">
+        <v>14.0</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8">
+        <v>29.952</v>
+      </c>
+      <c r="E15" s="8">
+        <v>21.634</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G15" s="8">
+        <v>18.638</v>
+      </c>
+      <c r="H15" s="8">
+        <v>4.478</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>18.638</v>
+      </c>
+      <c r="K15" s="8">
+        <v>4.478</v>
+      </c>
+      <c r="L15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M15" s="8">
+        <v>18.638</v>
+      </c>
+      <c r="N15" s="8">
+        <v>4.478</v>
+      </c>
+      <c r="O15" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P15" s="8">
+        <v>18.638</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>4.478</v>
+      </c>
+      <c r="R15" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="B16" s="8">
+        <v>15.0</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="8">
+        <v>9.918</v>
+      </c>
+      <c r="E16" s="8">
+        <v>2.359</v>
+      </c>
+      <c r="F16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G16" s="8">
+        <v>8.079</v>
+      </c>
+      <c r="H16" s="8">
+        <v>2.359</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>8.079</v>
+      </c>
+      <c r="K16" s="8">
+        <v>2.359</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M16" s="8">
+        <v>8.079</v>
+      </c>
+      <c r="N16" s="8">
+        <v>2.359</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>8.079</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>2.359</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="B17" s="8">
+        <v>16.0</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="8">
+        <v>9.519</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="F17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G17" s="8">
+        <v>9.519</v>
+      </c>
+      <c r="H17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>9.519</v>
+      </c>
+      <c r="K17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="L17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M17" s="8">
+        <v>9.519</v>
+      </c>
+      <c r="N17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="O17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P17" s="8">
+        <v>9.519</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="R17" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="B18" s="8">
+        <v>17.0</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="8">
+        <v>12.757</v>
+      </c>
+      <c r="E18" s="8">
+        <v>10.357</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G18" s="8">
+        <v>10.839</v>
+      </c>
+      <c r="H18" s="8">
+        <v>2.399</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>10.839</v>
+      </c>
+      <c r="K18" s="8">
+        <v>2.399</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M18" s="8">
+        <v>10.878</v>
+      </c>
+      <c r="N18" s="8">
+        <v>8.798</v>
+      </c>
+      <c r="O18" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P18" s="8">
+        <v>10.878</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>8.798</v>
+      </c>
+      <c r="R18" s="8">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="B19" s="8">
+        <v>18.0</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="8">
+        <v>5.117</v>
+      </c>
+      <c r="E19" s="8">
+        <v>6.237</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="G19" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="H19" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="J19" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="K19" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="M19" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="N19" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="O19" s="8">
+        <v>0.0</v>
+      </c>
+      <c r="P19" s="8">
+        <v>2.799</v>
+      </c>
+      <c r="Q19" s="8">
+        <v>4.998</v>
+      </c>
+      <c r="R19" s="8">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>